<commit_message>
Update some fixes conditions of error
</commit_message>
<xml_diff>
--- a/output/resultado_cartao_ponto.xlsx
+++ b/output/resultado_cartao_ponto.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="141">
   <si>
     <t>Data</t>
   </si>
@@ -815,7 +815,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M100"/>
+  <dimension ref="A1:M138"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
   </sheetViews>
@@ -2269,6 +2269,196 @@
         <v>113</v>
       </c>
     </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>132</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adicao mais informacoes cartaoPonto
</commit_message>
<xml_diff>
--- a/output/resultado_cartao_ponto.xlsx
+++ b/output/resultado_cartao_ponto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="89">
   <si>
     <t>Data</t>
   </si>
@@ -62,6 +62,12 @@
   </si>
   <si>
     <t>16:06</t>
+  </si>
+  <si>
+    <t>13:45</t>
+  </si>
+  <si>
+    <t>14:00</t>
   </si>
   <si>
     <t>S</t>
@@ -705,7 +711,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -718,122 +724,176 @@
       <c r="D2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
         <v>26</v>
       </c>
-      <c r="B6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" t="s">
-        <v>24</v>
-      </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D10" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
@@ -844,397 +904,571 @@
       <c r="D11" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D12" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D13" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D14" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" t="s">
         <v>46</v>
       </c>
-      <c r="D15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" t="s">
-        <v>44</v>
-      </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D16" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C18" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C19" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D19" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" t="s">
         <v>54</v>
       </c>
-      <c r="C20" t="s">
-        <v>55</v>
-      </c>
-      <c r="D20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>56</v>
-      </c>
-      <c r="B21" t="s">
-        <v>52</v>
-      </c>
       <c r="C21" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D21" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B22" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C22" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D22" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C23" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D23" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B24" t="s">
         <v>14</v>
       </c>
       <c r="C24" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D24" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C25" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D25" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>17</v>
+      </c>
+      <c r="F25" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B26" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C26" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D26" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B27" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C27" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D27" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>17</v>
+      </c>
+      <c r="F27" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B28" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C28" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D28" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>17</v>
+      </c>
+      <c r="F28" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B29" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C29" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D29" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>17</v>
+      </c>
+      <c r="F29" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B30" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C30" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D30" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>17</v>
+      </c>
+      <c r="F30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B31" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C31" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D31" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F31" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B32" t="s">
         <v>14</v>
       </c>
       <c r="C32" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D32" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>17</v>
+      </c>
+      <c r="F32" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B33" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C33" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D33" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>17</v>
+      </c>
+      <c r="F33" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B34" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C34" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D34" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>17</v>
+      </c>
+      <c r="F34" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>84</v>
+      </c>
+      <c r="B35" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" t="s">
+        <v>65</v>
+      </c>
+      <c r="D35" t="s">
+        <v>16</v>
+      </c>
+      <c r="E35" t="s">
+        <v>17</v>
+      </c>
+      <c r="F35" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>85</v>
+      </c>
+      <c r="B36" t="s">
+        <v>52</v>
+      </c>
+      <c r="C36" t="s">
         <v>82</v>
       </c>
-      <c r="B35" t="s">
-        <v>58</v>
-      </c>
-      <c r="C35" t="s">
-        <v>63</v>
-      </c>
-      <c r="D35" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>83</v>
-      </c>
-      <c r="B36" t="s">
-        <v>50</v>
-      </c>
-      <c r="C36" t="s">
-        <v>80</v>
-      </c>
       <c r="D36" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>17</v>
+      </c>
+      <c r="F36" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B37" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C37" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D37" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>17</v>
+      </c>
+      <c r="F37" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B38" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C38" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D38" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38" t="s">
+        <v>17</v>
+      </c>
+      <c r="F38" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B39" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C39" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D39" t="s">
         <v>16</v>
+      </c>
+      <c r="E39" t="s">
+        <v>17</v>
+      </c>
+      <c r="F39" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>